<commit_message>
Update to Figure 6
</commit_message>
<xml_diff>
--- a/Phase_Field_Fracture/Figures/3DNotchTest/Legend.xlsx
+++ b/Phase_Field_Fracture/Figures/3DNotchTest/Legend.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/idaang/Documents/GitHub/FEniCS/Phase_Field_Fracture/Figures/3DNotchTest/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{728D96B0-088D-BC45-89CA-8DCC62AD9113}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B015A1DB-C1F4-7847-89ED-6D28A883F6F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15860" yWindow="500" windowWidth="13040" windowHeight="14400" xr2:uid="{5584DDDF-2D1A-D34D-B615-DF937505A16D}"/>
+    <workbookView xWindow="16140" yWindow="620" windowWidth="13040" windowHeight="14400" xr2:uid="{5584DDDF-2D1A-D34D-B615-DF937505A16D}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -90,9 +90,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -407,10 +408,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E66A6E45-F927-B845-8D89-EAB3A2980D6C}">
-  <dimension ref="A1:E19"/>
+  <dimension ref="A1:E16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B20" sqref="B20"/>
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -432,11 +433,11 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A2">
-        <v>0.21</v>
+        <v>0.2</v>
       </c>
       <c r="B2">
         <f>A2/0.2</f>
-        <v>1.0499999999999998</v>
+        <v>1</v>
       </c>
       <c r="D2">
         <v>0.28000000000000003</v>
@@ -480,11 +481,11 @@
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5">
-        <v>5.0000000000000001E-3</v>
+        <v>0.05</v>
       </c>
       <c r="B5">
         <f t="shared" si="0"/>
-        <v>2.4999999999999998E-2</v>
+        <v>0.25</v>
       </c>
       <c r="D5">
         <v>0</v>
@@ -512,11 +513,11 @@
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7">
-        <v>-0.49</v>
+        <v>-0.44</v>
       </c>
       <c r="B7">
         <f t="shared" si="0"/>
-        <v>-2.4499999999999997</v>
+        <v>-2.1999999999999997</v>
       </c>
       <c r="D7">
         <v>-0.2</v>
@@ -559,11 +560,11 @@
         <v>8</v>
       </c>
       <c r="D10">
-        <v>2</v>
+        <v>1.9</v>
       </c>
       <c r="E10">
         <f>D10/0.2</f>
-        <v>10</v>
+        <v>9.4999999999999982</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
@@ -575,11 +576,11 @@
         <v>5</v>
       </c>
       <c r="D11">
-        <v>1.6</v>
+        <v>1.5</v>
       </c>
       <c r="E11">
         <f t="shared" ref="E11:E19" si="3">D11/0.2</f>
-        <v>8</v>
+        <v>7.5</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
@@ -591,11 +592,11 @@
         <v>2.5</v>
       </c>
       <c r="D12">
-        <v>1.4</v>
+        <v>1</v>
       </c>
       <c r="E12">
         <f t="shared" si="3"/>
-        <v>6.9999999999999991</v>
+        <v>5</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
@@ -607,11 +608,11 @@
         <v>0</v>
       </c>
       <c r="D13">
-        <v>1.2</v>
+        <v>0.5</v>
       </c>
       <c r="E13">
         <f t="shared" si="3"/>
-        <v>5.9999999999999991</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
@@ -622,12 +623,12 @@
         <f t="shared" si="2"/>
         <v>-2.5</v>
       </c>
-      <c r="D14">
-        <v>1</v>
+      <c r="D14" s="2">
+        <v>-9.1000000000000004E-3</v>
       </c>
       <c r="E14">
         <f t="shared" si="3"/>
-        <v>5</v>
+        <v>-4.5499999999999999E-2</v>
       </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
@@ -638,55 +639,14 @@
         <f t="shared" si="2"/>
         <v>-5</v>
       </c>
-      <c r="D15">
-        <v>0.8</v>
-      </c>
-      <c r="E15">
-        <f t="shared" si="3"/>
-        <v>4</v>
-      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16">
-        <v>-1.6</v>
+        <v>-1.5</v>
       </c>
       <c r="B16">
         <f t="shared" si="2"/>
-        <v>-8</v>
-      </c>
-      <c r="D16">
-        <v>0.6</v>
-      </c>
-      <c r="E16">
-        <f t="shared" si="3"/>
-        <v>2.9999999999999996</v>
-      </c>
-    </row>
-    <row r="17" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D17">
-        <v>0.4</v>
-      </c>
-      <c r="E17">
-        <f t="shared" si="3"/>
-        <v>2</v>
-      </c>
-    </row>
-    <row r="18" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D18">
-        <v>0.2</v>
-      </c>
-      <c r="E18">
-        <f t="shared" si="3"/>
-        <v>1</v>
-      </c>
-    </row>
-    <row r="19" spans="4:5" x14ac:dyDescent="0.2">
-      <c r="D19">
-        <v>-9.1000000000000004E-3</v>
-      </c>
-      <c r="E19">
-        <f t="shared" si="3"/>
-        <v>-4.5499999999999999E-2</v>
+        <v>-7.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>